<commit_message>
Resolução exercício aula 3
</commit_message>
<xml_diff>
--- a/Aula 2/Cenários de testes.xlsx
+++ b/Aula 2/Cenários de testes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Área de Trabalho\teste\EBAC_JornadaQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Área de Trabalho\teste\EBAC_JornadaQA\Aula 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122C9CD4-7D7A-4EF1-B90D-22B0F5E39C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F33446-04B7-4D08-B2A3-E2A8250D32D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3069688C-34A7-424E-9324-F52356C67A10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3069688C-34A7-424E-9324-F52356C67A10}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="102">
   <si>
     <t>US</t>
   </si>
@@ -438,7 +438,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -461,13 +461,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
@@ -481,32 +474,6 @@
           <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -840,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78D86B2-6D9D-49B0-B765-CA59F58AAB3B}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,7 +877,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>43</v>
@@ -1032,7 +999,7 @@
         <v>67</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1110,7 +1077,7 @@
         <v>43</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1162,7 +1129,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1188,7 +1155,7 @@
         <v>20</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1240,7 +1207,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1266,7 +1233,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1288,9 +1255,11 @@
       <c r="F16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="H16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1342,7 +1311,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1362,13 +1331,13 @@
         <v>51</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>52</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1498,7 +1467,7 @@
         <v>67</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1509,7 +1478,7 @@
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>$K$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1542,20 +1511,6 @@
             </x14:dxf>
           </x14:cfRule>
           <xm:sqref>H2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{877A235B-A71E-4158-BEAE-8551801AF9D2}">
-            <xm:f>NOT(ISERROR(SEARCH($K$2,H2)))</xm:f>
-            <xm:f>$K$2</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.24994659260841701"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H2:H20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="1" operator="containsText" id="{AACB5025-FAB7-4F93-A154-B048BD004FDF}">

</xml_diff>

<commit_message>
Refatoração testes - Aula 05
</commit_message>
<xml_diff>
--- a/Aula 2/Cenários de testes.xlsx
+++ b/Aula 2/Cenários de testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Área de Trabalho\teste\EBAC_JornadaQA\Aula 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65DDE1A-92FD-4C69-AACD-5516EB411761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C9ADDE-8192-47E3-8A9E-F2D68EC4D142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3069688C-34A7-424E-9324-F52356C67A10}"/>
   </bookViews>
@@ -449,6 +449,42 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
@@ -511,42 +547,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78D86B2-6D9D-49B0-B765-CA59F58AAB3B}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,23 +1631,23 @@
     </sortState>
   </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H2:I2 I2:I24">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>$L$2</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H3:H9">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20:H24">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>$L$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:I2 I2:I24">
+    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
       <formula>$L$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1667,59 +1667,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{0AD05D9D-8EF1-498F-84CA-3655CBFE26A9}">
-            <xm:f>NOT(ISERROR(SEARCH($L$2,H2)))</xm:f>
-            <xm:f>$L$2</xm:f>
-            <x14:dxf>
-              <font>
-                <color auto="1"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.24994659260841701"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H2:I2 I2:I24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{AACB5025-FAB7-4F93-A154-B048BD004FDF}">
-            <xm:f>NOT(ISERROR(SEARCH($L$4,I2)))</xm:f>
-            <xm:f>$L$4</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{200742D5-EBF8-4D0E-A7B9-BA4D3A3ECBBA}">
-            <xm:f>NOT(ISERROR(SEARCH($L$3,I2)))</xm:f>
-            <xm:f>$L$3</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{464F9BD2-DE5A-4867-9E68-DB5B525C144E}">
-            <xm:f>NOT(ISERROR(SEARCH($L$2,I2)))</xm:f>
-            <xm:f>$L$2</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="0" tint="-0.24994659260841701"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I2:I35</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="7" operator="containsText" id="{427B683D-0F9B-4ED0-BAF9-52CD86E34BE5}">
             <xm:f>NOT(ISERROR(SEARCH($L$4,H2)))</xm:f>
@@ -1807,6 +1754,59 @@
           </x14:cfRule>
           <xm:sqref>H20:H24</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{0AD05D9D-8EF1-498F-84CA-3655CBFE26A9}">
+            <xm:f>NOT(ISERROR(SEARCH($L$2,H2)))</xm:f>
+            <xm:f>$L$2</xm:f>
+            <x14:dxf>
+              <font>
+                <color auto="1"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.24994659260841701"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H2:I2 I2:I24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{AACB5025-FAB7-4F93-A154-B048BD004FDF}">
+            <xm:f>NOT(ISERROR(SEARCH($L$4,I2)))</xm:f>
+            <xm:f>$L$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{200742D5-EBF8-4D0E-A7B9-BA4D3A3ECBBA}">
+            <xm:f>NOT(ISERROR(SEARCH($L$3,I2)))</xm:f>
+            <xm:f>$L$3</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{464F9BD2-DE5A-4867-9E68-DB5B525C144E}">
+            <xm:f>NOT(ISERROR(SEARCH($L$2,I2)))</xm:f>
+            <xm:f>$L$2</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.24994659260841701"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2:I35</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>